<commit_message>
Update Qld_towns_RSQ pathways V2.xlsx
includes updated time for Springbrook from Adam
</commit_message>
<xml_diff>
--- a/input/drive_times/Qld_towns_RSQ pathways V2.xlsx
+++ b/input/drive_times/Qld_towns_RSQ pathways V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25301"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthqld.sharepoint.com/teams/TBIARIQ/Shared Documents/General/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4339" documentId="8_{E3C60C20-14D3-4F3F-84A3-022FA30A61C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46300977-0A8F-43CE-A8D6-E984939E0B61}"/>
+  <xr:revisionPtr revIDLastSave="4341" documentId="8_{E3C60C20-14D3-4F3F-84A3-022FA30A61C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6857420B-D975-4720-A089-1C60676899F6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5318,14 +5318,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{905C772C-C0DC-49BC-A1F9-D2C5730A00FE}" name="Table1" displayName="Table1" ref="A3:AB444" totalsRowShown="0">
-  <autoFilter ref="A3:AB444" xr:uid="{51D47EBF-65A8-4B57-A003-0A595E314FCB}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Injune"/>
-        <filter val="Miles"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:AB444" xr:uid="{51D47EBF-65A8-4B57-A003-0A595E314FCB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AB444">
     <sortCondition ref="Z3:Z444"/>
   </sortState>
@@ -5665,8 +5658,8 @@
   <dimension ref="A1:AB444"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="X445" sqref="X445"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="S17" sqref="S17"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -5817,7 +5810,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:28" hidden="1">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -5880,7 +5873,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:28" hidden="1">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -5943,7 +5936,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:28" hidden="1">
+    <row r="6" spans="1:28">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -6016,7 +6009,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:28" hidden="1">
+    <row r="7" spans="1:28">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -6082,7 +6075,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:28" hidden="1">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -6145,7 +6138,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:28" hidden="1">
+    <row r="9" spans="1:28">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -6211,7 +6204,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="1:28" hidden="1">
+    <row r="10" spans="1:28">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -6274,7 +6267,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:28" hidden="1">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -6337,7 +6330,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="12" spans="1:28" hidden="1">
+    <row r="12" spans="1:28">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -6400,7 +6393,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:28" hidden="1">
+    <row r="13" spans="1:28">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -6463,7 +6456,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:28" hidden="1">
+    <row r="14" spans="1:28">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -6526,7 +6519,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:28" hidden="1">
+    <row r="15" spans="1:28">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -6583,7 +6576,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:28" hidden="1">
+    <row r="16" spans="1:28">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -6646,7 +6639,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:28" hidden="1">
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
         <v>93</v>
       </c>
@@ -6686,15 +6679,18 @@
       <c r="P17">
         <v>15</v>
       </c>
+      <c r="R17">
+        <v>46</v>
+      </c>
       <c r="T17" t="s">
         <v>99</v>
       </c>
       <c r="AB17">
         <f>SUM(Table1[[#This Row],[Coordination_time_mins]:[Aeromdical_scene_1_time_mins]])+ SUM(Table1[[#This Row],[Aircraft2_response_time_mins]:[Destination_road_time_mins]])</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" hidden="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -6749,7 +6745,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:28" hidden="1">
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -6806,7 +6802,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:28" hidden="1">
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>107</v>
       </c>
@@ -6872,7 +6868,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="21" spans="1:28" hidden="1">
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -6927,7 +6923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:28" hidden="1">
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
         <v>114</v>
       </c>
@@ -6990,7 +6986,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:28" hidden="1">
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -7057,7 +7053,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:28" hidden="1">
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -7109,7 +7105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:28" hidden="1">
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -7166,7 +7162,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:28" hidden="1">
+    <row r="26" spans="1:28">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -7232,7 +7228,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:28" hidden="1">
+    <row r="27" spans="1:28">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -7287,7 +7283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:28" hidden="1">
+    <row r="28" spans="1:28">
       <c r="A28" t="s">
         <v>136</v>
       </c>
@@ -7342,7 +7338,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:28" hidden="1">
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -7397,7 +7393,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:28" hidden="1">
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -7452,7 +7448,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:28" hidden="1">
+    <row r="31" spans="1:28">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -7507,7 +7503,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:28" hidden="1">
+    <row r="32" spans="1:28">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -7562,7 +7558,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:28" hidden="1">
+    <row r="33" spans="1:28">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -7617,7 +7613,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:28" hidden="1">
+    <row r="34" spans="1:28">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -7674,7 +7670,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:28" hidden="1">
+    <row r="35" spans="1:28">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -7729,7 +7725,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:28" hidden="1">
+    <row r="36" spans="1:28">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -7796,7 +7792,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="37" spans="1:28" hidden="1">
+    <row r="37" spans="1:28">
       <c r="A37" t="s">
         <v>163</v>
       </c>
@@ -7851,7 +7847,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:28" hidden="1">
+    <row r="38" spans="1:28">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -7903,7 +7899,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:28" hidden="1">
+    <row r="39" spans="1:28">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -7958,7 +7954,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:28" hidden="1">
+    <row r="40" spans="1:28">
       <c r="A40" t="s">
         <v>172</v>
       </c>
@@ -8022,7 +8018,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:28" hidden="1">
+    <row r="41" spans="1:28">
       <c r="A41" t="s">
         <v>176</v>
       </c>
@@ -8077,7 +8073,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:28" hidden="1">
+    <row r="42" spans="1:28">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -8132,7 +8128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:28" hidden="1">
+    <row r="43" spans="1:28">
       <c r="A43" t="s">
         <v>182</v>
       </c>
@@ -8187,7 +8183,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:28" hidden="1">
+    <row r="44" spans="1:28">
       <c r="A44" t="s">
         <v>185</v>
       </c>
@@ -8242,7 +8238,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:28" hidden="1">
+    <row r="45" spans="1:28">
       <c r="A45" t="s">
         <v>188</v>
       </c>
@@ -8297,7 +8293,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:28" hidden="1">
+    <row r="46" spans="1:28">
       <c r="A46" t="s">
         <v>191</v>
       </c>
@@ -8352,7 +8348,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:28" hidden="1">
+    <row r="47" spans="1:28">
       <c r="A47" t="s">
         <v>194</v>
       </c>
@@ -8419,7 +8415,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:28" hidden="1">
+    <row r="48" spans="1:28">
       <c r="A48" t="s">
         <v>197</v>
       </c>
@@ -8474,7 +8470,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:28" hidden="1">
+    <row r="49" spans="1:28">
       <c r="A49" t="s">
         <v>200</v>
       </c>
@@ -8529,7 +8525,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:28" hidden="1">
+    <row r="50" spans="1:28">
       <c r="A50" t="s">
         <v>203</v>
       </c>
@@ -8584,7 +8580,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:28" hidden="1">
+    <row r="51" spans="1:28">
       <c r="A51" t="s">
         <v>206</v>
       </c>
@@ -8651,7 +8647,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:28" hidden="1">
+    <row r="52" spans="1:28">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -8718,7 +8714,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:28" hidden="1">
+    <row r="53" spans="1:28">
       <c r="A53" t="s">
         <v>212</v>
       </c>
@@ -8773,7 +8769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:28" hidden="1">
+    <row r="54" spans="1:28">
       <c r="A54" t="s">
         <v>215</v>
       </c>
@@ -8830,7 +8826,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:28" hidden="1">
+    <row r="55" spans="1:28">
       <c r="A55" t="s">
         <v>218</v>
       </c>
@@ -8897,7 +8893,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:28" hidden="1">
+    <row r="56" spans="1:28">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -8952,7 +8948,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:28" hidden="1">
+    <row r="57" spans="1:28">
       <c r="A57" t="s">
         <v>224</v>
       </c>
@@ -9019,7 +9015,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:28" hidden="1">
+    <row r="58" spans="1:28">
       <c r="A58" t="s">
         <v>227</v>
       </c>
@@ -9076,7 +9072,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:28" hidden="1">
+    <row r="59" spans="1:28">
       <c r="A59" t="s">
         <v>230</v>
       </c>
@@ -9131,7 +9127,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:28" hidden="1">
+    <row r="60" spans="1:28">
       <c r="A60" t="s">
         <v>233</v>
       </c>
@@ -9186,7 +9182,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:28" hidden="1">
+    <row r="61" spans="1:28">
       <c r="A61" t="s">
         <v>236</v>
       </c>
@@ -9243,7 +9239,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:28" hidden="1">
+    <row r="62" spans="1:28">
       <c r="A62" t="s">
         <v>239</v>
       </c>
@@ -9298,7 +9294,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:28" hidden="1">
+    <row r="63" spans="1:28">
       <c r="A63" t="s">
         <v>242</v>
       </c>
@@ -9355,7 +9351,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:28" hidden="1">
+    <row r="64" spans="1:28">
       <c r="A64" t="s">
         <v>245</v>
       </c>
@@ -9422,7 +9418,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:28" hidden="1">
+    <row r="65" spans="1:28">
       <c r="A65" t="s">
         <v>248</v>
       </c>
@@ -9489,7 +9485,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:28" hidden="1">
+    <row r="66" spans="1:28">
       <c r="A66" t="s">
         <v>251</v>
       </c>
@@ -9544,7 +9540,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:28" hidden="1">
+    <row r="67" spans="1:28">
       <c r="A67" t="s">
         <v>254</v>
       </c>
@@ -9601,7 +9597,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:28" hidden="1">
+    <row r="68" spans="1:28">
       <c r="A68" t="s">
         <v>257</v>
       </c>
@@ -9656,7 +9652,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:28" hidden="1">
+    <row r="69" spans="1:28">
       <c r="A69" t="s">
         <v>260</v>
       </c>
@@ -9711,7 +9707,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:28" hidden="1">
+    <row r="70" spans="1:28">
       <c r="A70" t="s">
         <v>263</v>
       </c>
@@ -9768,7 +9764,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:28" hidden="1">
+    <row r="71" spans="1:28">
       <c r="A71" t="s">
         <v>266</v>
       </c>
@@ -9823,7 +9819,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:28" hidden="1">
+    <row r="72" spans="1:28">
       <c r="A72" t="s">
         <v>269</v>
       </c>
@@ -9880,7 +9876,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="1:28" hidden="1">
+    <row r="73" spans="1:28">
       <c r="A73" t="s">
         <v>272</v>
       </c>
@@ -9947,7 +9943,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:28" hidden="1">
+    <row r="74" spans="1:28">
       <c r="A74" t="s">
         <v>275</v>
       </c>
@@ -10004,7 +10000,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:28" hidden="1">
+    <row r="75" spans="1:28">
       <c r="A75" t="s">
         <v>278</v>
       </c>
@@ -10061,7 +10057,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="1:28" hidden="1">
+    <row r="76" spans="1:28">
       <c r="A76" t="s">
         <v>281</v>
       </c>
@@ -10128,7 +10124,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="1:28" hidden="1">
+    <row r="77" spans="1:28">
       <c r="A77" t="s">
         <v>284</v>
       </c>
@@ -10195,7 +10191,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:28" hidden="1">
+    <row r="78" spans="1:28">
       <c r="A78" t="s">
         <v>287</v>
       </c>
@@ -10262,7 +10258,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:28" hidden="1">
+    <row r="79" spans="1:28">
       <c r="A79" t="s">
         <v>290</v>
       </c>
@@ -10319,7 +10315,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="80" spans="1:28" hidden="1">
+    <row r="80" spans="1:28">
       <c r="A80" t="s">
         <v>293</v>
       </c>
@@ -10376,7 +10372,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:28" hidden="1">
+    <row r="81" spans="1:28">
       <c r="A81" t="s">
         <v>296</v>
       </c>
@@ -10431,7 +10427,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:28" hidden="1">
+    <row r="82" spans="1:28">
       <c r="A82" t="s">
         <v>299</v>
       </c>
@@ -10498,7 +10494,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:28" hidden="1">
+    <row r="83" spans="1:28">
       <c r="A83" t="s">
         <v>302</v>
       </c>
@@ -10553,7 +10549,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="1:28" hidden="1">
+    <row r="84" spans="1:28">
       <c r="A84" t="s">
         <v>305</v>
       </c>
@@ -10620,7 +10616,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="1:28" hidden="1">
+    <row r="85" spans="1:28">
       <c r="A85" t="s">
         <v>308</v>
       </c>
@@ -10687,7 +10683,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="86" spans="1:28" hidden="1">
+    <row r="86" spans="1:28">
       <c r="A86" t="s">
         <v>311</v>
       </c>
@@ -10744,7 +10740,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:28" hidden="1">
+    <row r="87" spans="1:28">
       <c r="A87" t="s">
         <v>314</v>
       </c>
@@ -10799,7 +10795,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:28" hidden="1">
+    <row r="88" spans="1:28">
       <c r="A88" t="s">
         <v>317</v>
       </c>
@@ -10866,7 +10862,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:28" hidden="1">
+    <row r="89" spans="1:28">
       <c r="A89" t="s">
         <v>320</v>
       </c>
@@ -10933,7 +10929,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:28" hidden="1">
+    <row r="90" spans="1:28">
       <c r="A90" t="s">
         <v>323</v>
       </c>
@@ -10985,7 +10981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:28" hidden="1">
+    <row r="91" spans="1:28">
       <c r="A91" t="s">
         <v>327</v>
       </c>
@@ -11052,7 +11048,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="92" spans="1:28" hidden="1">
+    <row r="92" spans="1:28">
       <c r="A92" t="s">
         <v>330</v>
       </c>
@@ -11119,7 +11115,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="93" spans="1:28" hidden="1">
+    <row r="93" spans="1:28">
       <c r="A93" t="s">
         <v>333</v>
       </c>
@@ -11174,7 +11170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="94" spans="1:28" hidden="1">
+    <row r="94" spans="1:28">
       <c r="A94" t="s">
         <v>336</v>
       </c>
@@ -11231,7 +11227,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:28" hidden="1">
+    <row r="95" spans="1:28">
       <c r="A95" t="s">
         <v>339</v>
       </c>
@@ -11298,7 +11294,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="96" spans="1:28" hidden="1">
+    <row r="96" spans="1:28">
       <c r="A96" t="s">
         <v>342</v>
       </c>
@@ -11355,7 +11351,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="97" spans="1:28" hidden="1">
+    <row r="97" spans="1:28">
       <c r="A97" t="s">
         <v>345</v>
       </c>
@@ -11422,7 +11418,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:28" hidden="1">
+    <row r="98" spans="1:28">
       <c r="A98" t="s">
         <v>348</v>
       </c>
@@ -11489,7 +11485,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:28" hidden="1">
+    <row r="99" spans="1:28">
       <c r="A99" t="s">
         <v>351</v>
       </c>
@@ -11546,7 +11542,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="100" spans="1:28" hidden="1">
+    <row r="100" spans="1:28">
       <c r="A100" t="s">
         <v>354</v>
       </c>
@@ -11603,7 +11599,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:28" hidden="1">
+    <row r="101" spans="1:28">
       <c r="A101" t="s">
         <v>357</v>
       </c>
@@ -11658,7 +11654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:28" hidden="1">
+    <row r="102" spans="1:28">
       <c r="A102" t="s">
         <v>360</v>
       </c>
@@ -11713,7 +11709,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:28" hidden="1">
+    <row r="103" spans="1:28">
       <c r="A103" t="s">
         <v>363</v>
       </c>
@@ -11768,7 +11764,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="104" spans="1:28" hidden="1">
+    <row r="104" spans="1:28">
       <c r="A104" t="s">
         <v>366</v>
       </c>
@@ -11823,7 +11819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:28" hidden="1">
+    <row r="105" spans="1:28">
       <c r="A105" t="s">
         <v>369</v>
       </c>
@@ -11886,7 +11882,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="106" spans="1:28" hidden="1">
+    <row r="106" spans="1:28">
       <c r="A106" t="s">
         <v>373</v>
       </c>
@@ -11953,7 +11949,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="107" spans="1:28" hidden="1">
+    <row r="107" spans="1:28">
       <c r="A107" t="s">
         <v>376</v>
       </c>
@@ -12010,7 +12006,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="108" spans="1:28" hidden="1">
+    <row r="108" spans="1:28">
       <c r="A108" t="s">
         <v>379</v>
       </c>
@@ -12065,7 +12061,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:28" hidden="1">
+    <row r="109" spans="1:28">
       <c r="A109" t="s">
         <v>382</v>
       </c>
@@ -12129,7 +12125,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="110" spans="1:28" hidden="1">
+    <row r="110" spans="1:28">
       <c r="A110" t="s">
         <v>386</v>
       </c>
@@ -12196,7 +12192,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="111" spans="1:28" hidden="1">
+    <row r="111" spans="1:28">
       <c r="A111" t="s">
         <v>390</v>
       </c>
@@ -12251,7 +12247,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="112" spans="1:28" hidden="1">
+    <row r="112" spans="1:28">
       <c r="A112" t="s">
         <v>393</v>
       </c>
@@ -12308,7 +12304,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="113" spans="1:28" hidden="1">
+    <row r="113" spans="1:28">
       <c r="A113" t="s">
         <v>396</v>
       </c>
@@ -12363,7 +12359,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="1:28" hidden="1">
+    <row r="114" spans="1:28">
       <c r="A114" t="s">
         <v>399</v>
       </c>
@@ -12418,7 +12414,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="115" spans="1:28" hidden="1">
+    <row r="115" spans="1:28">
       <c r="A115" t="s">
         <v>402</v>
       </c>
@@ -12473,7 +12469,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="116" spans="1:28" hidden="1">
+    <row r="116" spans="1:28">
       <c r="A116" t="s">
         <v>405</v>
       </c>
@@ -12528,7 +12524,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="117" spans="1:28" hidden="1">
+    <row r="117" spans="1:28">
       <c r="A117" t="s">
         <v>408</v>
       </c>
@@ -12583,7 +12579,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:28" hidden="1">
+    <row r="118" spans="1:28">
       <c r="A118" t="s">
         <v>411</v>
       </c>
@@ -12638,7 +12634,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:28" hidden="1">
+    <row r="119" spans="1:28">
       <c r="A119" t="s">
         <v>414</v>
       </c>
@@ -12693,7 +12689,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="120" spans="1:28" hidden="1">
+    <row r="120" spans="1:28">
       <c r="A120" t="s">
         <v>417</v>
       </c>
@@ -12748,7 +12744,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="121" spans="1:28" hidden="1">
+    <row r="121" spans="1:28">
       <c r="A121" t="s">
         <v>420</v>
       </c>
@@ -12803,7 +12799,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="122" spans="1:28" hidden="1">
+    <row r="122" spans="1:28">
       <c r="A122" t="s">
         <v>423</v>
       </c>
@@ -12858,7 +12854,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="123" spans="1:28" hidden="1">
+    <row r="123" spans="1:28">
       <c r="A123" t="s">
         <v>426</v>
       </c>
@@ -12913,7 +12909,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="124" spans="1:28" hidden="1">
+    <row r="124" spans="1:28">
       <c r="A124" t="s">
         <v>429</v>
       </c>
@@ -12970,7 +12966,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="125" spans="1:28" hidden="1">
+    <row r="125" spans="1:28">
       <c r="A125" t="s">
         <v>433</v>
       </c>
@@ -13025,7 +13021,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="126" spans="1:28" hidden="1">
+    <row r="126" spans="1:28">
       <c r="A126" t="s">
         <v>436</v>
       </c>
@@ -13088,7 +13084,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="127" spans="1:28" hidden="1">
+    <row r="127" spans="1:28">
       <c r="A127" t="s">
         <v>439</v>
       </c>
@@ -13143,7 +13139,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:28" hidden="1">
+    <row r="128" spans="1:28">
       <c r="A128" t="s">
         <v>442</v>
       </c>
@@ -13206,7 +13202,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="129" spans="1:28" hidden="1">
+    <row r="129" spans="1:28">
       <c r="A129" t="s">
         <v>446</v>
       </c>
@@ -13263,7 +13259,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="130" spans="1:28" hidden="1">
+    <row r="130" spans="1:28">
       <c r="A130" t="s">
         <v>449</v>
       </c>
@@ -13320,7 +13316,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="131" spans="1:28" hidden="1">
+    <row r="131" spans="1:28">
       <c r="A131" t="s">
         <v>452</v>
       </c>
@@ -13383,7 +13379,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="132" spans="1:28" hidden="1">
+    <row r="132" spans="1:28">
       <c r="A132" t="s">
         <v>455</v>
       </c>
@@ -13450,7 +13446,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="133" spans="1:28" hidden="1">
+    <row r="133" spans="1:28">
       <c r="A133" t="s">
         <v>459</v>
       </c>
@@ -13516,7 +13512,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="134" spans="1:28" hidden="1">
+    <row r="134" spans="1:28">
       <c r="A134" t="s">
         <v>463</v>
       </c>
@@ -13583,7 +13579,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="135" spans="1:28" hidden="1">
+    <row r="135" spans="1:28">
       <c r="A135" t="s">
         <v>466</v>
       </c>
@@ -13650,7 +13646,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:28" hidden="1">
+    <row r="136" spans="1:28">
       <c r="A136" t="s">
         <v>469</v>
       </c>
@@ -13707,7 +13703,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="137" spans="1:28" hidden="1">
+    <row r="137" spans="1:28">
       <c r="A137" t="s">
         <v>472</v>
       </c>
@@ -13773,7 +13769,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="138" spans="1:28" hidden="1">
+    <row r="138" spans="1:28">
       <c r="A138" t="s">
         <v>477</v>
       </c>
@@ -13840,7 +13836,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="139" spans="1:28" hidden="1">
+    <row r="139" spans="1:28">
       <c r="A139" t="s">
         <v>480</v>
       </c>
@@ -13907,7 +13903,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="140" spans="1:28" hidden="1">
+    <row r="140" spans="1:28">
       <c r="A140" t="s">
         <v>483</v>
       </c>
@@ -13970,7 +13966,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:28" hidden="1">
+    <row r="141" spans="1:28">
       <c r="A141" t="s">
         <v>486</v>
       </c>
@@ -14104,7 +14100,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="143" spans="1:28" ht="21.6" hidden="1" customHeight="1">
+    <row r="143" spans="1:28" ht="21.6" customHeight="1">
       <c r="A143" t="s">
         <v>493</v>
       </c>
@@ -14171,7 +14167,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="144" spans="1:28" s="13" customFormat="1" hidden="1">
+    <row r="144" spans="1:28" s="13" customFormat="1">
       <c r="A144" t="s">
         <v>496</v>
       </c>
@@ -14244,7 +14240,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="145" spans="1:28" hidden="1">
+    <row r="145" spans="1:28">
       <c r="A145" t="s">
         <v>499</v>
       </c>
@@ -14311,7 +14307,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="1:28" hidden="1">
+    <row r="146" spans="1:28">
       <c r="A146" t="s">
         <v>502</v>
       </c>
@@ -14368,7 +14364,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="147" spans="1:28" hidden="1">
+    <row r="147" spans="1:28">
       <c r="A147" t="s">
         <v>505</v>
       </c>
@@ -14435,7 +14431,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="148" spans="1:28" hidden="1">
+    <row r="148" spans="1:28">
       <c r="A148" t="s">
         <v>509</v>
       </c>
@@ -14502,7 +14498,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="149" spans="1:28" hidden="1">
+    <row r="149" spans="1:28">
       <c r="A149" t="s">
         <v>513</v>
       </c>
@@ -14559,7 +14555,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="150" spans="1:28" hidden="1">
+    <row r="150" spans="1:28">
       <c r="A150" t="s">
         <v>516</v>
       </c>
@@ -14616,7 +14612,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="151" spans="1:28" hidden="1">
+    <row r="151" spans="1:28">
       <c r="A151" t="s">
         <v>519</v>
       </c>
@@ -14683,7 +14679,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="152" spans="1:28" hidden="1">
+    <row r="152" spans="1:28">
       <c r="A152" t="s">
         <v>522</v>
       </c>
@@ -14750,7 +14746,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="153" spans="1:28" hidden="1">
+    <row r="153" spans="1:28">
       <c r="A153" t="s">
         <v>525</v>
       </c>
@@ -14817,7 +14813,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="154" spans="1:28" hidden="1">
+    <row r="154" spans="1:28">
       <c r="A154" t="s">
         <v>528</v>
       </c>
@@ -14881,7 +14877,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="155" spans="1:28" hidden="1">
+    <row r="155" spans="1:28">
       <c r="A155" t="s">
         <v>532</v>
       </c>
@@ -14948,7 +14944,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="156" spans="1:28" hidden="1">
+    <row r="156" spans="1:28">
       <c r="A156" t="s">
         <v>536</v>
       </c>
@@ -15015,7 +15011,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="157" spans="1:28" hidden="1">
+    <row r="157" spans="1:28">
       <c r="A157" t="s">
         <v>539</v>
       </c>
@@ -15072,7 +15068,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="158" spans="1:28" hidden="1">
+    <row r="158" spans="1:28">
       <c r="A158" t="s">
         <v>542</v>
       </c>
@@ -15139,7 +15135,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:28" hidden="1">
+    <row r="159" spans="1:28">
       <c r="A159" t="s">
         <v>545</v>
       </c>
@@ -15206,7 +15202,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:28" hidden="1">
+    <row r="160" spans="1:28">
       <c r="A160" t="s">
         <v>548</v>
       </c>
@@ -15273,7 +15269,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="161" spans="1:28" hidden="1">
+    <row r="161" spans="1:28">
       <c r="A161" t="s">
         <v>551</v>
       </c>
@@ -15340,7 +15336,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="162" spans="1:28" hidden="1">
+    <row r="162" spans="1:28">
       <c r="A162" t="s">
         <v>554</v>
       </c>
@@ -15407,7 +15403,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="163" spans="1:28" hidden="1">
+    <row r="163" spans="1:28">
       <c r="A163" t="s">
         <v>558</v>
       </c>
@@ -15474,7 +15470,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="164" spans="1:28" hidden="1">
+    <row r="164" spans="1:28">
       <c r="A164" t="s">
         <v>561</v>
       </c>
@@ -15531,7 +15527,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="165" spans="1:28" hidden="1">
+    <row r="165" spans="1:28">
       <c r="A165" t="s">
         <v>564</v>
       </c>
@@ -15598,7 +15594,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="166" spans="1:28" hidden="1">
+    <row r="166" spans="1:28">
       <c r="A166" t="s">
         <v>567</v>
       </c>
@@ -15665,7 +15661,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="167" spans="1:28" hidden="1">
+    <row r="167" spans="1:28">
       <c r="A167" t="s">
         <v>570</v>
       </c>
@@ -15722,7 +15718,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="168" spans="1:28" hidden="1">
+    <row r="168" spans="1:28">
       <c r="A168" t="s">
         <v>573</v>
       </c>
@@ -15779,7 +15775,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="169" spans="1:28" hidden="1">
+    <row r="169" spans="1:28">
       <c r="A169" t="s">
         <v>576</v>
       </c>
@@ -15842,7 +15838,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="170" spans="1:28" hidden="1">
+    <row r="170" spans="1:28">
       <c r="A170" t="s">
         <v>579</v>
       </c>
@@ -15905,7 +15901,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171" spans="1:28" hidden="1">
+    <row r="171" spans="1:28">
       <c r="A171" t="s">
         <v>583</v>
       </c>
@@ -15962,7 +15958,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="172" spans="1:28" hidden="1">
+    <row r="172" spans="1:28">
       <c r="A172" t="s">
         <v>586</v>
       </c>
@@ -16025,7 +16021,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="1:28" hidden="1">
+    <row r="173" spans="1:28">
       <c r="A173" t="s">
         <v>590</v>
       </c>
@@ -16089,7 +16085,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="174" spans="1:28" hidden="1">
+    <row r="174" spans="1:28">
       <c r="A174" t="s">
         <v>594</v>
       </c>
@@ -16156,7 +16152,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="175" spans="1:28" hidden="1">
+    <row r="175" spans="1:28">
       <c r="A175" t="s">
         <v>597</v>
       </c>
@@ -16220,7 +16216,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="176" spans="1:28" hidden="1">
+    <row r="176" spans="1:28">
       <c r="A176" t="s">
         <v>600</v>
       </c>
@@ -16284,7 +16280,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="177" spans="1:28" hidden="1">
+    <row r="177" spans="1:28">
       <c r="A177" t="s">
         <v>603</v>
       </c>
@@ -16348,7 +16344,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="178" spans="1:28" hidden="1">
+    <row r="178" spans="1:28">
       <c r="A178" t="s">
         <v>606</v>
       </c>
@@ -16412,7 +16408,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:28" hidden="1">
+    <row r="179" spans="1:28">
       <c r="A179" t="s">
         <v>609</v>
       </c>
@@ -16476,7 +16472,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="180" spans="1:28" hidden="1">
+    <row r="180" spans="1:28">
       <c r="A180" t="s">
         <v>612</v>
       </c>
@@ -16543,7 +16539,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="181" spans="1:28" hidden="1">
+    <row r="181" spans="1:28">
       <c r="A181" t="s">
         <v>615</v>
       </c>
@@ -16600,7 +16596,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="182" spans="1:28" hidden="1">
+    <row r="182" spans="1:28">
       <c r="A182" t="s">
         <v>618</v>
       </c>
@@ -16667,7 +16663,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="183" spans="1:28" hidden="1">
+    <row r="183" spans="1:28">
       <c r="A183" t="s">
         <v>621</v>
       </c>
@@ -16724,7 +16720,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="184" spans="1:28" hidden="1">
+    <row r="184" spans="1:28">
       <c r="A184" t="s">
         <v>624</v>
       </c>
@@ -16791,7 +16787,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="185" spans="1:28" hidden="1">
+    <row r="185" spans="1:28">
       <c r="A185" t="s">
         <v>628</v>
       </c>
@@ -16848,7 +16844,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="186" spans="1:28" hidden="1">
+    <row r="186" spans="1:28">
       <c r="A186" t="s">
         <v>631</v>
       </c>
@@ -16905,7 +16901,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="187" spans="1:28" hidden="1">
+    <row r="187" spans="1:28">
       <c r="A187" t="s">
         <v>634</v>
       </c>
@@ -17039,7 +17035,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="189" spans="1:28" hidden="1">
+    <row r="189" spans="1:28">
       <c r="A189" t="s">
         <v>641</v>
       </c>
@@ -17105,7 +17101,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="190" spans="1:28" hidden="1">
+    <row r="190" spans="1:28">
       <c r="A190" t="s">
         <v>645</v>
       </c>
@@ -17172,7 +17168,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="191" spans="1:28" hidden="1">
+    <row r="191" spans="1:28">
       <c r="A191" t="s">
         <v>648</v>
       </c>
@@ -17229,7 +17225,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="192" spans="1:28" hidden="1">
+    <row r="192" spans="1:28">
       <c r="A192" t="s">
         <v>651</v>
       </c>
@@ -17296,7 +17292,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="193" spans="1:28" hidden="1">
+    <row r="193" spans="1:28">
       <c r="A193" t="s">
         <v>654</v>
       </c>
@@ -17360,7 +17356,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="194" spans="1:28" hidden="1">
+    <row r="194" spans="1:28">
       <c r="A194" t="s">
         <v>657</v>
       </c>
@@ -17423,7 +17419,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="195" spans="1:28" hidden="1">
+    <row r="195" spans="1:28">
       <c r="A195" t="s">
         <v>661</v>
       </c>
@@ -17490,7 +17486,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="196" spans="1:28" hidden="1">
+    <row r="196" spans="1:28">
       <c r="A196" t="s">
         <v>664</v>
       </c>
@@ -17553,7 +17549,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="197" spans="1:28" hidden="1">
+    <row r="197" spans="1:28">
       <c r="A197" t="s">
         <v>668</v>
       </c>
@@ -17620,7 +17616,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="198" spans="1:28" hidden="1">
+    <row r="198" spans="1:28">
       <c r="A198" t="s">
         <v>671</v>
       </c>
@@ -17687,7 +17683,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="199" spans="1:28" hidden="1">
+    <row r="199" spans="1:28">
       <c r="A199" t="s">
         <v>674</v>
       </c>
@@ -17747,7 +17743,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="200" spans="1:28" hidden="1">
+    <row r="200" spans="1:28">
       <c r="A200" t="s">
         <v>678</v>
       </c>
@@ -17814,7 +17810,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="201" spans="1:28" hidden="1">
+    <row r="201" spans="1:28">
       <c r="A201" t="s">
         <v>681</v>
       </c>
@@ -17881,7 +17877,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="202" spans="1:28" hidden="1">
+    <row r="202" spans="1:28">
       <c r="A202" t="s">
         <v>684</v>
       </c>
@@ -17944,7 +17940,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="203" spans="1:28" hidden="1">
+    <row r="203" spans="1:28">
       <c r="A203" t="s">
         <v>688</v>
       </c>
@@ -18011,7 +18007,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:28" hidden="1">
+    <row r="204" spans="1:28">
       <c r="A204" t="s">
         <v>691</v>
       </c>
@@ -18078,7 +18074,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="205" spans="1:28" hidden="1">
+    <row r="205" spans="1:28">
       <c r="A205" t="s">
         <v>694</v>
       </c>
@@ -18145,7 +18141,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="206" spans="1:28" hidden="1">
+    <row r="206" spans="1:28">
       <c r="A206" t="s">
         <v>697</v>
       </c>
@@ -18212,7 +18208,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="207" spans="1:28" hidden="1">
+    <row r="207" spans="1:28">
       <c r="A207" t="s">
         <v>700</v>
       </c>
@@ -18279,7 +18275,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="208" spans="1:28" hidden="1">
+    <row r="208" spans="1:28">
       <c r="A208" t="s">
         <v>703</v>
       </c>
@@ -18346,7 +18342,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="209" spans="1:28" hidden="1">
+    <row r="209" spans="1:28">
       <c r="A209" t="s">
         <v>706</v>
       </c>
@@ -18413,7 +18409,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="210" spans="1:28" hidden="1">
+    <row r="210" spans="1:28">
       <c r="A210" t="s">
         <v>709</v>
       </c>
@@ -18480,7 +18476,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="211" spans="1:28" hidden="1">
+    <row r="211" spans="1:28">
       <c r="A211" t="s">
         <v>712</v>
       </c>
@@ -18547,7 +18543,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="212" spans="1:28" hidden="1">
+    <row r="212" spans="1:28">
       <c r="A212" t="s">
         <v>716</v>
       </c>
@@ -18614,7 +18610,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="1:28" hidden="1">
+    <row r="213" spans="1:28">
       <c r="A213" t="s">
         <v>719</v>
       </c>
@@ -18681,7 +18677,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="214" spans="1:28" hidden="1">
+    <row r="214" spans="1:28">
       <c r="A214" t="s">
         <v>722</v>
       </c>
@@ -18748,7 +18744,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="215" spans="1:28" hidden="1">
+    <row r="215" spans="1:28">
       <c r="A215" t="s">
         <v>725</v>
       </c>
@@ -18815,7 +18811,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="216" spans="1:28" hidden="1">
+    <row r="216" spans="1:28">
       <c r="A216" t="s">
         <v>728</v>
       </c>
@@ -18872,7 +18868,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="217" spans="1:28" hidden="1">
+    <row r="217" spans="1:28">
       <c r="A217" t="s">
         <v>731</v>
       </c>
@@ -18939,7 +18935,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="218" spans="1:28" hidden="1">
+    <row r="218" spans="1:28">
       <c r="A218" t="s">
         <v>734</v>
       </c>
@@ -19006,7 +19002,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="219" spans="1:28" hidden="1">
+    <row r="219" spans="1:28">
       <c r="A219" t="s">
         <v>737</v>
       </c>
@@ -19073,7 +19069,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="220" spans="1:28" hidden="1">
+    <row r="220" spans="1:28">
       <c r="A220" t="s">
         <v>740</v>
       </c>
@@ -19140,7 +19136,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="221" spans="1:28" hidden="1">
+    <row r="221" spans="1:28">
       <c r="A221" t="s">
         <v>743</v>
       </c>
@@ -19203,7 +19199,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="222" spans="1:28" hidden="1">
+    <row r="222" spans="1:28">
       <c r="A222" t="s">
         <v>747</v>
       </c>
@@ -19270,7 +19266,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="223" spans="1:28" hidden="1">
+    <row r="223" spans="1:28">
       <c r="A223" t="s">
         <v>750</v>
       </c>
@@ -19337,7 +19333,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="224" spans="1:28" hidden="1">
+    <row r="224" spans="1:28">
       <c r="A224" t="s">
         <v>753</v>
       </c>
@@ -19403,7 +19399,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="225" spans="1:28" hidden="1">
+    <row r="225" spans="1:28">
       <c r="A225" t="s">
         <v>757</v>
       </c>
@@ -19470,7 +19466,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="226" spans="1:28" hidden="1">
+    <row r="226" spans="1:28">
       <c r="A226" t="s">
         <v>760</v>
       </c>
@@ -19537,7 +19533,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="227" spans="1:28" hidden="1">
+    <row r="227" spans="1:28">
       <c r="A227" t="s">
         <v>763</v>
       </c>
@@ -19601,7 +19597,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="228" spans="1:28" hidden="1">
+    <row r="228" spans="1:28">
       <c r="A228" t="s">
         <v>767</v>
       </c>
@@ -19668,7 +19664,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="229" spans="1:28" hidden="1">
+    <row r="229" spans="1:28">
       <c r="A229" t="s">
         <v>242</v>
       </c>
@@ -19735,7 +19731,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="230" spans="1:28" hidden="1">
+    <row r="230" spans="1:28">
       <c r="A230" t="s">
         <v>771</v>
       </c>
@@ -19802,7 +19798,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="231" spans="1:28" hidden="1">
+    <row r="231" spans="1:28">
       <c r="A231" t="s">
         <v>774</v>
       </c>
@@ -19869,7 +19865,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="232" spans="1:28" hidden="1">
+    <row r="232" spans="1:28">
       <c r="A232" t="s">
         <v>777</v>
       </c>
@@ -19936,7 +19932,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="233" spans="1:28" hidden="1">
+    <row r="233" spans="1:28">
       <c r="A233" t="s">
         <v>780</v>
       </c>
@@ -20003,7 +19999,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="234" spans="1:28" hidden="1">
+    <row r="234" spans="1:28">
       <c r="A234" t="s">
         <v>783</v>
       </c>
@@ -20067,7 +20063,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="235" spans="1:28" hidden="1">
+    <row r="235" spans="1:28">
       <c r="A235" t="s">
         <v>787</v>
       </c>
@@ -20131,7 +20127,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="236" spans="1:28" hidden="1">
+    <row r="236" spans="1:28">
       <c r="A236" t="s">
         <v>791</v>
       </c>
@@ -20198,7 +20194,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="237" spans="1:28" hidden="1">
+    <row r="237" spans="1:28">
       <c r="A237" t="s">
         <v>794</v>
       </c>
@@ -20262,7 +20258,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="238" spans="1:28" hidden="1">
+    <row r="238" spans="1:28">
       <c r="A238" t="s">
         <v>797</v>
       </c>
@@ -20319,7 +20315,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="239" spans="1:28" hidden="1">
+    <row r="239" spans="1:28">
       <c r="A239" t="s">
         <v>800</v>
       </c>
@@ -20386,7 +20382,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="240" spans="1:28" hidden="1">
+    <row r="240" spans="1:28">
       <c r="A240" t="s">
         <v>804</v>
       </c>
@@ -20458,7 +20454,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="241" spans="1:28" hidden="1">
+    <row r="241" spans="1:28">
       <c r="A241" t="s">
         <v>808</v>
       </c>
@@ -20525,7 +20521,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="242" spans="1:28" hidden="1">
+    <row r="242" spans="1:28">
       <c r="A242" t="s">
         <v>812</v>
       </c>
@@ -20597,7 +20593,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="243" spans="1:28" hidden="1">
+    <row r="243" spans="1:28">
       <c r="A243" t="s">
         <v>815</v>
       </c>
@@ -20663,7 +20659,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="244" spans="1:28" hidden="1">
+    <row r="244" spans="1:28">
       <c r="A244" t="s">
         <v>818</v>
       </c>
@@ -20730,7 +20726,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="245" spans="1:28" hidden="1">
+    <row r="245" spans="1:28">
       <c r="A245" t="s">
         <v>822</v>
       </c>
@@ -20794,7 +20790,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="246" spans="1:28" hidden="1">
+    <row r="246" spans="1:28">
       <c r="A246" t="s">
         <v>826</v>
       </c>
@@ -20857,7 +20853,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="247" spans="1:28" hidden="1">
+    <row r="247" spans="1:28">
       <c r="A247" t="s">
         <v>829</v>
       </c>
@@ -20921,7 +20917,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="248" spans="1:28" hidden="1">
+    <row r="248" spans="1:28">
       <c r="A248" t="s">
         <v>832</v>
       </c>
@@ -20985,7 +20981,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="249" spans="1:28" hidden="1">
+    <row r="249" spans="1:28">
       <c r="A249" t="s">
         <v>835</v>
       </c>
@@ -21048,7 +21044,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="250" spans="1:28" hidden="1">
+    <row r="250" spans="1:28">
       <c r="A250" t="s">
         <v>838</v>
       </c>
@@ -21118,7 +21114,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="251" spans="1:28" hidden="1">
+    <row r="251" spans="1:28">
       <c r="A251" t="s">
         <v>842</v>
       </c>
@@ -21184,7 +21180,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="252" spans="1:28" hidden="1">
+    <row r="252" spans="1:28">
       <c r="A252" t="s">
         <v>846</v>
       </c>
@@ -21254,7 +21250,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="253" spans="1:28" hidden="1">
+    <row r="253" spans="1:28">
       <c r="A253" t="s">
         <v>849</v>
       </c>
@@ -21321,7 +21317,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="254" spans="1:28" hidden="1">
+    <row r="254" spans="1:28">
       <c r="A254" t="s">
         <v>853</v>
       </c>
@@ -21387,7 +21383,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="255" spans="1:28" hidden="1">
+    <row r="255" spans="1:28">
       <c r="A255" t="s">
         <v>857</v>
       </c>
@@ -21457,7 +21453,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="256" spans="1:28" hidden="1">
+    <row r="256" spans="1:28">
       <c r="A256" t="s">
         <v>860</v>
       </c>
@@ -21523,7 +21519,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="257" spans="1:28" hidden="1">
+    <row r="257" spans="1:28">
       <c r="A257" t="s">
         <v>863</v>
       </c>
@@ -21593,7 +21589,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="258" spans="1:28" hidden="1">
+    <row r="258" spans="1:28">
       <c r="A258" t="s">
         <v>866</v>
       </c>
@@ -21660,7 +21656,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="259" spans="1:28" hidden="1">
+    <row r="259" spans="1:28">
       <c r="A259" t="s">
         <v>869</v>
       </c>
@@ -21726,7 +21722,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="260" spans="1:28" hidden="1">
+    <row r="260" spans="1:28">
       <c r="A260" t="s">
         <v>873</v>
       </c>
@@ -21792,7 +21788,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="261" spans="1:28" hidden="1">
+    <row r="261" spans="1:28">
       <c r="A261" t="s">
         <v>876</v>
       </c>
@@ -21859,7 +21855,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="262" spans="1:28" hidden="1">
+    <row r="262" spans="1:28">
       <c r="A262" t="s">
         <v>879</v>
       </c>
@@ -21925,7 +21921,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="263" spans="1:28" hidden="1">
+    <row r="263" spans="1:28">
       <c r="A263" t="s">
         <v>883</v>
       </c>
@@ -21995,7 +21991,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="264" spans="1:28" hidden="1">
+    <row r="264" spans="1:28">
       <c r="A264" t="s">
         <v>886</v>
       </c>
@@ -22061,7 +22057,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="265" spans="1:28" hidden="1">
+    <row r="265" spans="1:28">
       <c r="A265" t="s">
         <v>889</v>
       </c>
@@ -22131,7 +22127,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="266" spans="1:28" hidden="1">
+    <row r="266" spans="1:28">
       <c r="A266" t="s">
         <v>892</v>
       </c>
@@ -22201,7 +22197,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="267" spans="1:28" hidden="1">
+    <row r="267" spans="1:28">
       <c r="A267" t="s">
         <v>895</v>
       </c>
@@ -22271,7 +22267,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="268" spans="1:28" hidden="1">
+    <row r="268" spans="1:28">
       <c r="A268" t="s">
         <v>898</v>
       </c>
@@ -22341,7 +22337,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="269" spans="1:28" hidden="1">
+    <row r="269" spans="1:28">
       <c r="A269" t="s">
         <v>902</v>
       </c>
@@ -22411,7 +22407,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="270" spans="1:28" hidden="1">
+    <row r="270" spans="1:28">
       <c r="A270" t="s">
         <v>905</v>
       </c>
@@ -22481,7 +22477,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="271" spans="1:28" hidden="1">
+    <row r="271" spans="1:28">
       <c r="A271" t="s">
         <v>908</v>
       </c>
@@ -22551,7 +22547,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="272" spans="1:28" hidden="1">
+    <row r="272" spans="1:28">
       <c r="A272" t="s">
         <v>911</v>
       </c>
@@ -22621,7 +22617,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="273" spans="1:28" hidden="1">
+    <row r="273" spans="1:28">
       <c r="A273" t="s">
         <v>914</v>
       </c>
@@ -22687,7 +22683,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="274" spans="1:28" hidden="1">
+    <row r="274" spans="1:28">
       <c r="A274" t="s">
         <v>917</v>
       </c>
@@ -22762,7 +22758,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="275" spans="1:28" hidden="1">
+    <row r="275" spans="1:28">
       <c r="A275" t="s">
         <v>920</v>
       </c>
@@ -22828,7 +22824,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="276" spans="1:28" hidden="1">
+    <row r="276" spans="1:28">
       <c r="A276" t="s">
         <v>923</v>
       </c>
@@ -22903,7 +22899,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="277" spans="1:28" hidden="1">
+    <row r="277" spans="1:28">
       <c r="A277" t="s">
         <v>928</v>
       </c>
@@ -22973,7 +22969,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="278" spans="1:28" hidden="1">
+    <row r="278" spans="1:28">
       <c r="A278" t="s">
         <v>931</v>
       </c>
@@ -23045,7 +23041,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="279" spans="1:28" hidden="1">
+    <row r="279" spans="1:28">
       <c r="A279" t="s">
         <v>935</v>
       </c>
@@ -23117,7 +23113,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="280" spans="1:28" hidden="1">
+    <row r="280" spans="1:28">
       <c r="A280" t="s">
         <v>939</v>
       </c>
@@ -23189,7 +23185,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="281" spans="1:28" hidden="1">
+    <row r="281" spans="1:28">
       <c r="A281" t="s">
         <v>942</v>
       </c>
@@ -23264,7 +23260,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="282" spans="1:28" hidden="1">
+    <row r="282" spans="1:28">
       <c r="A282" t="s">
         <v>947</v>
       </c>
@@ -23336,7 +23332,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="283" spans="1:28" hidden="1">
+    <row r="283" spans="1:28">
       <c r="A283" t="s">
         <v>951</v>
       </c>
@@ -23409,7 +23405,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="284" spans="1:28" hidden="1">
+    <row r="284" spans="1:28">
       <c r="A284" t="s">
         <v>955</v>
       </c>
@@ -23482,7 +23478,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="285" spans="1:28" hidden="1">
+    <row r="285" spans="1:28">
       <c r="A285" t="s">
         <v>958</v>
       </c>
@@ -23555,7 +23551,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="286" spans="1:28" hidden="1">
+    <row r="286" spans="1:28">
       <c r="A286" t="s">
         <v>961</v>
       </c>
@@ -23628,7 +23624,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="287" spans="1:28" hidden="1">
+    <row r="287" spans="1:28">
       <c r="A287" t="s">
         <v>964</v>
       </c>
@@ -23701,7 +23697,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="288" spans="1:28" hidden="1">
+    <row r="288" spans="1:28">
       <c r="A288" t="s">
         <v>967</v>
       </c>
@@ -23774,7 +23770,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="289" spans="1:28" hidden="1">
+    <row r="289" spans="1:28">
       <c r="A289" t="s">
         <v>970</v>
       </c>
@@ -23834,7 +23830,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="290" spans="1:28" hidden="1">
+    <row r="290" spans="1:28">
       <c r="A290" t="s">
         <v>973</v>
       </c>
@@ -23907,7 +23903,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="291" spans="1:28" hidden="1">
+    <row r="291" spans="1:28">
       <c r="A291" t="s">
         <v>976</v>
       </c>
@@ -23980,7 +23976,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="292" spans="1:28" hidden="1">
+    <row r="292" spans="1:28">
       <c r="A292" t="s">
         <v>979</v>
       </c>
@@ -24053,7 +24049,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="293" spans="1:28" hidden="1">
+    <row r="293" spans="1:28">
       <c r="A293" t="s">
         <v>982</v>
       </c>
@@ -24126,7 +24122,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="294" spans="1:28" hidden="1">
+    <row r="294" spans="1:28">
       <c r="A294" t="s">
         <v>985</v>
       </c>
@@ -24199,7 +24195,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="295" spans="1:28" hidden="1">
+    <row r="295" spans="1:28">
       <c r="A295" t="s">
         <v>988</v>
       </c>
@@ -24272,7 +24268,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="296" spans="1:28" hidden="1">
+    <row r="296" spans="1:28">
       <c r="A296" t="s">
         <v>991</v>
       </c>
@@ -24345,7 +24341,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="297" spans="1:28" hidden="1">
+    <row r="297" spans="1:28">
       <c r="A297" t="s">
         <v>994</v>
       </c>
@@ -24418,7 +24414,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="298" spans="1:28" hidden="1">
+    <row r="298" spans="1:28">
       <c r="A298" t="s">
         <v>997</v>
       </c>
@@ -24491,7 +24487,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="299" spans="1:28" hidden="1">
+    <row r="299" spans="1:28">
       <c r="A299" t="s">
         <v>1000</v>
       </c>
@@ -24564,7 +24560,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="300" spans="1:28" hidden="1">
+    <row r="300" spans="1:28">
       <c r="A300" t="s">
         <v>1003</v>
       </c>
@@ -24637,7 +24633,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="301" spans="1:28" hidden="1">
+    <row r="301" spans="1:28">
       <c r="A301" s="13" t="s">
         <v>1006</v>
       </c>
@@ -24708,7 +24704,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="302" spans="1:28" hidden="1">
+    <row r="302" spans="1:28">
       <c r="A302" t="s">
         <v>1008</v>
       </c>
@@ -24781,7 +24777,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="303" spans="1:28" hidden="1">
+    <row r="303" spans="1:28">
       <c r="A303" t="s">
         <v>1011</v>
       </c>
@@ -24854,7 +24850,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="304" spans="1:28" hidden="1">
+    <row r="304" spans="1:28">
       <c r="A304" t="s">
         <v>1014</v>
       </c>
@@ -24927,7 +24923,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="305" spans="1:28" hidden="1">
+    <row r="305" spans="1:28">
       <c r="A305" t="s">
         <v>1017</v>
       </c>
@@ -25002,7 +24998,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="306" spans="1:28" hidden="1">
+    <row r="306" spans="1:28">
       <c r="A306" t="s">
         <v>1022</v>
       </c>
@@ -25077,7 +25073,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="307" spans="1:28" hidden="1">
+    <row r="307" spans="1:28">
       <c r="A307" t="s">
         <v>1026</v>
       </c>
@@ -25152,7 +25148,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="308" spans="1:28" hidden="1">
+    <row r="308" spans="1:28">
       <c r="A308" t="s">
         <v>1030</v>
       </c>
@@ -25227,7 +25223,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="309" spans="1:28" hidden="1">
+    <row r="309" spans="1:28">
       <c r="A309" t="s">
         <v>1034</v>
       </c>
@@ -25302,7 +25298,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="310" spans="1:28" hidden="1">
+    <row r="310" spans="1:28">
       <c r="A310" t="s">
         <v>1038</v>
       </c>
@@ -25375,7 +25371,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="311" spans="1:28" hidden="1">
+    <row r="311" spans="1:28">
       <c r="A311" t="s">
         <v>1041</v>
       </c>
@@ -25439,7 +25435,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="312" spans="1:28" hidden="1">
+    <row r="312" spans="1:28">
       <c r="A312" t="s">
         <v>1045</v>
       </c>
@@ -25505,7 +25501,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="313" spans="1:28" hidden="1">
+    <row r="313" spans="1:28">
       <c r="A313" t="s">
         <v>1048</v>
       </c>
@@ -25574,7 +25570,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="314" spans="1:28" hidden="1">
+    <row r="314" spans="1:28">
       <c r="A314" t="s">
         <v>1052</v>
       </c>
@@ -25643,7 +25639,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="315" spans="1:28" hidden="1">
+    <row r="315" spans="1:28">
       <c r="A315" t="s">
         <v>1055</v>
       </c>
@@ -25703,7 +25699,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="316" spans="1:28" hidden="1">
+    <row r="316" spans="1:28">
       <c r="A316" t="s">
         <v>1058</v>
       </c>
@@ -25772,7 +25768,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="317" spans="1:28" hidden="1">
+    <row r="317" spans="1:28">
       <c r="A317" t="s">
         <v>1061</v>
       </c>
@@ -25841,7 +25837,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="318" spans="1:28" hidden="1">
+    <row r="318" spans="1:28">
       <c r="A318" t="s">
         <v>1064</v>
       </c>
@@ -25901,7 +25897,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="319" spans="1:28" hidden="1">
+    <row r="319" spans="1:28">
       <c r="A319" t="s">
         <v>1067</v>
       </c>
@@ -25970,7 +25966,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="320" spans="1:28" hidden="1">
+    <row r="320" spans="1:28">
       <c r="A320" t="s">
         <v>1070</v>
       </c>
@@ -26042,7 +26038,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="321" spans="1:28" hidden="1">
+    <row r="321" spans="1:28">
       <c r="A321" t="s">
         <v>1074</v>
       </c>
@@ -26114,7 +26110,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="322" spans="1:28" hidden="1">
+    <row r="322" spans="1:28">
       <c r="A322" t="s">
         <v>1078</v>
       </c>
@@ -26186,7 +26182,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="323" spans="1:28" hidden="1">
+    <row r="323" spans="1:28">
       <c r="A323" t="s">
         <v>1081</v>
       </c>
@@ -26261,7 +26257,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="324" spans="1:28" hidden="1">
+    <row r="324" spans="1:28">
       <c r="A324" t="s">
         <v>1085</v>
       </c>
@@ -26333,7 +26329,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="325" spans="1:28" hidden="1">
+    <row r="325" spans="1:28">
       <c r="A325" t="s">
         <v>1089</v>
       </c>
@@ -26405,7 +26401,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="326" spans="1:28" hidden="1">
+    <row r="326" spans="1:28">
       <c r="A326" t="s">
         <v>1092</v>
       </c>
@@ -26477,7 +26473,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="327" spans="1:28" hidden="1">
+    <row r="327" spans="1:28">
       <c r="A327" t="s">
         <v>486</v>
       </c>
@@ -26549,7 +26545,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="328" spans="1:28" hidden="1">
+    <row r="328" spans="1:28">
       <c r="A328" t="s">
         <v>1096</v>
       </c>
@@ -26604,7 +26600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="329" spans="1:28" hidden="1">
+    <row r="329" spans="1:28">
       <c r="A329" t="s">
         <v>1099</v>
       </c>
@@ -26664,7 +26660,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="330" spans="1:28" hidden="1">
+    <row r="330" spans="1:28">
       <c r="A330" t="s">
         <v>1102</v>
       </c>
@@ -26719,7 +26715,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="331" spans="1:28" hidden="1">
+    <row r="331" spans="1:28">
       <c r="A331" t="s">
         <v>1105</v>
       </c>
@@ -26774,7 +26770,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="332" spans="1:28" hidden="1">
+    <row r="332" spans="1:28">
       <c r="A332" t="s">
         <v>1108</v>
       </c>
@@ -26829,7 +26825,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="333" spans="1:28" hidden="1">
+    <row r="333" spans="1:28">
       <c r="A333" t="s">
         <v>1111</v>
       </c>
@@ -26884,7 +26880,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="334" spans="1:28" hidden="1">
+    <row r="334" spans="1:28">
       <c r="A334" t="s">
         <v>1114</v>
       </c>
@@ -26939,7 +26935,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="335" spans="1:28" hidden="1">
+    <row r="335" spans="1:28">
       <c r="A335" t="s">
         <v>1117</v>
       </c>
@@ -26994,7 +26990,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="336" spans="1:28" hidden="1">
+    <row r="336" spans="1:28">
       <c r="A336" t="s">
         <v>1120</v>
       </c>
@@ -27049,7 +27045,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="337" spans="1:28" hidden="1">
+    <row r="337" spans="1:28">
       <c r="A337" t="s">
         <v>1123</v>
       </c>
@@ -27104,7 +27100,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="338" spans="1:28" hidden="1">
+    <row r="338" spans="1:28">
       <c r="A338" t="s">
         <v>1126</v>
       </c>
@@ -27159,7 +27155,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="339" spans="1:28" hidden="1">
+    <row r="339" spans="1:28">
       <c r="A339" t="s">
         <v>1129</v>
       </c>
@@ -27214,7 +27210,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="340" spans="1:28" hidden="1">
+    <row r="340" spans="1:28">
       <c r="A340" t="s">
         <v>1132</v>
       </c>
@@ -27274,7 +27270,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="341" spans="1:28" hidden="1">
+    <row r="341" spans="1:28">
       <c r="A341" t="s">
         <v>1135</v>
       </c>
@@ -27329,7 +27325,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="342" spans="1:28" hidden="1">
+    <row r="342" spans="1:28">
       <c r="A342" t="s">
         <v>1138</v>
       </c>
@@ -27384,7 +27380,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="343" spans="1:28" hidden="1">
+    <row r="343" spans="1:28">
       <c r="A343" t="s">
         <v>1141</v>
       </c>
@@ -27444,7 +27440,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="344" spans="1:28" hidden="1">
+    <row r="344" spans="1:28">
       <c r="A344" t="s">
         <v>1144</v>
       </c>
@@ -27504,7 +27500,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="345" spans="1:28" hidden="1">
+    <row r="345" spans="1:28">
       <c r="A345" t="s">
         <v>1147</v>
       </c>
@@ -27559,7 +27555,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="346" spans="1:28" hidden="1">
+    <row r="346" spans="1:28">
       <c r="A346" t="s">
         <v>1150</v>
       </c>
@@ -27619,7 +27615,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="347" spans="1:28" hidden="1">
+    <row r="347" spans="1:28">
       <c r="A347" t="s">
         <v>1153</v>
       </c>
@@ -27674,7 +27670,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="348" spans="1:28" hidden="1">
+    <row r="348" spans="1:28">
       <c r="A348" t="s">
         <v>1156</v>
       </c>
@@ -27746,7 +27742,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="349" spans="1:28" hidden="1">
+    <row r="349" spans="1:28">
       <c r="A349" t="s">
         <v>1160</v>
       </c>
@@ -27818,7 +27814,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="350" spans="1:28" hidden="1">
+    <row r="350" spans="1:28">
       <c r="A350" t="s">
         <v>1164</v>
       </c>
@@ -27890,7 +27886,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="351" spans="1:28" hidden="1">
+    <row r="351" spans="1:28">
       <c r="A351" t="s">
         <v>1168</v>
       </c>
@@ -27962,7 +27958,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="352" spans="1:28" hidden="1">
+    <row r="352" spans="1:28">
       <c r="A352" t="s">
         <v>1171</v>
       </c>
@@ -28034,7 +28030,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="353" spans="1:28" hidden="1">
+    <row r="353" spans="1:28">
       <c r="A353" t="s">
         <v>1174</v>
       </c>
@@ -28106,7 +28102,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="354" spans="1:28" hidden="1">
+    <row r="354" spans="1:28">
       <c r="A354" t="s">
         <v>1177</v>
       </c>
@@ -28178,7 +28174,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="355" spans="1:28" hidden="1">
+    <row r="355" spans="1:28">
       <c r="A355" t="s">
         <v>1180</v>
       </c>
@@ -28250,7 +28246,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="356" spans="1:28" hidden="1">
+    <row r="356" spans="1:28">
       <c r="A356" t="s">
         <v>1183</v>
       </c>
@@ -28325,7 +28321,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="357" spans="1:28" hidden="1">
+    <row r="357" spans="1:28">
       <c r="A357" t="s">
         <v>1187</v>
       </c>
@@ -28397,7 +28393,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="358" spans="1:28" hidden="1">
+    <row r="358" spans="1:28">
       <c r="A358" t="s">
         <v>1190</v>
       </c>
@@ -28472,7 +28468,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="359" spans="1:28" hidden="1">
+    <row r="359" spans="1:28">
       <c r="A359" t="s">
         <v>1194</v>
       </c>
@@ -28544,7 +28540,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="360" spans="1:28" hidden="1">
+    <row r="360" spans="1:28">
       <c r="A360" t="s">
         <v>1198</v>
       </c>
@@ -28616,7 +28612,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="361" spans="1:28" hidden="1">
+    <row r="361" spans="1:28">
       <c r="A361" t="s">
         <v>1201</v>
       </c>
@@ -28688,7 +28684,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="362" spans="1:28" hidden="1">
+    <row r="362" spans="1:28">
       <c r="A362" t="s">
         <v>1204</v>
       </c>
@@ -28763,7 +28759,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="363" spans="1:28" hidden="1">
+    <row r="363" spans="1:28">
       <c r="A363" t="s">
         <v>1208</v>
       </c>
@@ -28835,7 +28831,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="364" spans="1:28" hidden="1">
+    <row r="364" spans="1:28">
       <c r="A364" t="s">
         <v>1211</v>
       </c>
@@ -28907,7 +28903,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="365" spans="1:28" hidden="1">
+    <row r="365" spans="1:28">
       <c r="A365" t="s">
         <v>1214</v>
       </c>
@@ -28979,7 +28975,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="366" spans="1:28" hidden="1">
+    <row r="366" spans="1:28">
       <c r="A366" t="s">
         <v>1217</v>
       </c>
@@ -29051,7 +29047,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="367" spans="1:28" hidden="1">
+    <row r="367" spans="1:28">
       <c r="A367" t="s">
         <v>1220</v>
       </c>
@@ -29123,7 +29119,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="368" spans="1:28" hidden="1">
+    <row r="368" spans="1:28">
       <c r="A368" t="s">
         <v>1223</v>
       </c>
@@ -29195,7 +29191,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="369" spans="1:28" hidden="1">
+    <row r="369" spans="1:28">
       <c r="A369" t="s">
         <v>1227</v>
       </c>
@@ -29267,7 +29263,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="370" spans="1:28" hidden="1">
+    <row r="370" spans="1:28">
       <c r="A370" t="s">
         <v>1230</v>
       </c>
@@ -29342,7 +29338,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="371" spans="1:28" hidden="1">
+    <row r="371" spans="1:28">
       <c r="A371" t="s">
         <v>1234</v>
       </c>
@@ -29402,7 +29398,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="372" spans="1:28" hidden="1">
+    <row r="372" spans="1:28">
       <c r="A372" t="s">
         <v>1237</v>
       </c>
@@ -29477,7 +29473,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="373" spans="1:28" hidden="1">
+    <row r="373" spans="1:28">
       <c r="A373" t="s">
         <v>1242</v>
       </c>
@@ -29549,7 +29545,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="374" spans="1:28" hidden="1">
+    <row r="374" spans="1:28">
       <c r="A374" t="s">
         <v>1246</v>
       </c>
@@ -29621,7 +29617,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="375" spans="1:28" hidden="1">
+    <row r="375" spans="1:28">
       <c r="A375" t="s">
         <v>1249</v>
       </c>
@@ -29693,7 +29689,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="376" spans="1:28" hidden="1">
+    <row r="376" spans="1:28">
       <c r="A376" t="s">
         <v>1252</v>
       </c>
@@ -29765,7 +29761,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="377" spans="1:28" hidden="1">
+    <row r="377" spans="1:28">
       <c r="A377" t="s">
         <v>1255</v>
       </c>
@@ -29837,7 +29833,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="378" spans="1:28" hidden="1">
+    <row r="378" spans="1:28">
       <c r="A378" t="s">
         <v>1258</v>
       </c>
@@ -29909,7 +29905,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="379" spans="1:28" hidden="1">
+    <row r="379" spans="1:28">
       <c r="A379" t="s">
         <v>1261</v>
       </c>
@@ -29981,7 +29977,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="380" spans="1:28" hidden="1">
+    <row r="380" spans="1:28">
       <c r="A380" t="s">
         <v>1264</v>
       </c>
@@ -30053,7 +30049,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="381" spans="1:28" hidden="1">
+    <row r="381" spans="1:28">
       <c r="A381" t="s">
         <v>1267</v>
       </c>
@@ -30125,7 +30121,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="382" spans="1:28" hidden="1">
+    <row r="382" spans="1:28">
       <c r="A382" t="s">
         <v>1270</v>
       </c>
@@ -30200,7 +30196,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="383" spans="1:28" hidden="1">
+    <row r="383" spans="1:28">
       <c r="A383" t="s">
         <v>1273</v>
       </c>
@@ -30272,7 +30268,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="384" spans="1:28" hidden="1">
+    <row r="384" spans="1:28">
       <c r="A384" t="s">
         <v>1276</v>
       </c>
@@ -30345,7 +30341,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="385" spans="1:28" hidden="1">
+    <row r="385" spans="1:28">
       <c r="A385" t="s">
         <v>1279</v>
       </c>
@@ -30417,7 +30413,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="386" spans="1:28" hidden="1">
+    <row r="386" spans="1:28">
       <c r="A386" t="s">
         <v>1283</v>
       </c>
@@ -30489,7 +30485,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="387" spans="1:28" hidden="1">
+    <row r="387" spans="1:28">
       <c r="A387" t="s">
         <v>1286</v>
       </c>
@@ -30561,7 +30557,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="388" spans="1:28" hidden="1">
+    <row r="388" spans="1:28">
       <c r="A388" t="s">
         <v>1290</v>
       </c>
@@ -30634,7 +30630,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="389" spans="1:28" hidden="1">
+    <row r="389" spans="1:28">
       <c r="A389" t="s">
         <v>1293</v>
       </c>
@@ -30706,7 +30702,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="390" spans="1:28" hidden="1">
+    <row r="390" spans="1:28">
       <c r="A390" t="s">
         <v>1296</v>
       </c>
@@ -30778,7 +30774,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="391" spans="1:28" hidden="1">
+    <row r="391" spans="1:28">
       <c r="A391" t="s">
         <v>1299</v>
       </c>
@@ -30850,7 +30846,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="392" spans="1:28" hidden="1">
+    <row r="392" spans="1:28">
       <c r="A392" t="s">
         <v>1302</v>
       </c>
@@ -30922,7 +30918,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="393" spans="1:28" hidden="1">
+    <row r="393" spans="1:28">
       <c r="A393" t="s">
         <v>1305</v>
       </c>
@@ -30994,7 +30990,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="394" spans="1:28" hidden="1">
+    <row r="394" spans="1:28">
       <c r="A394" t="s">
         <v>1308</v>
       </c>
@@ -31066,7 +31062,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="395" spans="1:28" hidden="1">
+    <row r="395" spans="1:28">
       <c r="A395" t="s">
         <v>1312</v>
       </c>
@@ -31138,7 +31134,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="396" spans="1:28" hidden="1">
+    <row r="396" spans="1:28">
       <c r="A396" t="s">
         <v>1316</v>
       </c>
@@ -31198,7 +31194,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="397" spans="1:28" hidden="1">
+    <row r="397" spans="1:28">
       <c r="A397" t="s">
         <v>1319</v>
       </c>
@@ -31271,7 +31267,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="398" spans="1:28" hidden="1">
+    <row r="398" spans="1:28">
       <c r="A398" t="s">
         <v>1322</v>
       </c>
@@ -31344,7 +31340,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="399" spans="1:28" hidden="1">
+    <row r="399" spans="1:28">
       <c r="A399" t="s">
         <v>1325</v>
       </c>
@@ -31414,7 +31410,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="400" spans="1:28" hidden="1">
+    <row r="400" spans="1:28">
       <c r="A400" t="s">
         <v>1328</v>
       </c>
@@ -31484,7 +31480,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="401" spans="1:28" hidden="1">
+    <row r="401" spans="1:28">
       <c r="A401" t="s">
         <v>1330</v>
       </c>
@@ -31557,7 +31553,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="402" spans="1:28" hidden="1">
+    <row r="402" spans="1:28">
       <c r="A402" t="s">
         <v>1333</v>
       </c>
@@ -31627,7 +31623,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="403" spans="1:28" hidden="1">
+    <row r="403" spans="1:28">
       <c r="A403" t="s">
         <v>1337</v>
       </c>
@@ -31700,7 +31696,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="404" spans="1:28" hidden="1">
+    <row r="404" spans="1:28">
       <c r="A404" t="s">
         <v>1340</v>
       </c>
@@ -31773,7 +31769,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="405" spans="1:28" hidden="1">
+    <row r="405" spans="1:28">
       <c r="A405" t="s">
         <v>1344</v>
       </c>
@@ -31846,7 +31842,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="406" spans="1:28" hidden="1">
+    <row r="406" spans="1:28">
       <c r="A406" t="s">
         <v>1347</v>
       </c>
@@ -31919,7 +31915,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="407" spans="1:28" hidden="1">
+    <row r="407" spans="1:28">
       <c r="A407" t="s">
         <v>1350</v>
       </c>
@@ -31991,7 +31987,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="408" spans="1:28" hidden="1">
+    <row r="408" spans="1:28">
       <c r="A408" t="s">
         <v>1354</v>
       </c>
@@ -32063,7 +32059,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="409" spans="1:28" hidden="1">
+    <row r="409" spans="1:28">
       <c r="A409" t="s">
         <v>1357</v>
       </c>
@@ -32135,7 +32131,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="410" spans="1:28" hidden="1">
+    <row r="410" spans="1:28">
       <c r="A410" t="s">
         <v>1360</v>
       </c>
@@ -32207,7 +32203,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="411" spans="1:28" hidden="1">
+    <row r="411" spans="1:28">
       <c r="A411" t="s">
         <v>1363</v>
       </c>
@@ -32279,7 +32275,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="412" spans="1:28" hidden="1">
+    <row r="412" spans="1:28">
       <c r="A412" t="s">
         <v>1366</v>
       </c>
@@ -32351,7 +32347,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="413" spans="1:28" hidden="1">
+    <row r="413" spans="1:28">
       <c r="A413" t="s">
         <v>1369</v>
       </c>
@@ -32423,7 +32419,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="414" spans="1:28" hidden="1">
+    <row r="414" spans="1:28">
       <c r="A414" t="s">
         <v>1373</v>
       </c>
@@ -32498,7 +32494,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="415" spans="1:28" hidden="1">
+    <row r="415" spans="1:28">
       <c r="A415" t="s">
         <v>1377</v>
       </c>
@@ -32570,7 +32566,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="416" spans="1:28" hidden="1">
+    <row r="416" spans="1:28">
       <c r="A416" t="s">
         <v>1381</v>
       </c>
@@ -32642,7 +32638,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="417" spans="1:28" hidden="1">
+    <row r="417" spans="1:28">
       <c r="A417" t="s">
         <v>1385</v>
       </c>
@@ -32717,7 +32713,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="418" spans="1:28" hidden="1">
+    <row r="418" spans="1:28">
       <c r="A418" t="s">
         <v>1389</v>
       </c>
@@ -32792,7 +32788,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="419" spans="1:28" hidden="1">
+    <row r="419" spans="1:28">
       <c r="A419" t="s">
         <v>1393</v>
       </c>
@@ -32867,7 +32863,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="420" spans="1:28" hidden="1">
+    <row r="420" spans="1:28">
       <c r="A420" t="s">
         <v>1397</v>
       </c>
@@ -32942,7 +32938,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="421" spans="1:28" hidden="1">
+    <row r="421" spans="1:28">
       <c r="A421" t="s">
         <v>1401</v>
       </c>
@@ -33017,7 +33013,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="422" spans="1:28" hidden="1">
+    <row r="422" spans="1:28">
       <c r="A422" t="s">
         <v>1405</v>
       </c>
@@ -33092,7 +33088,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="423" spans="1:28" hidden="1">
+    <row r="423" spans="1:28">
       <c r="A423" t="s">
         <v>1407</v>
       </c>
@@ -33167,7 +33163,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="424" spans="1:28" hidden="1">
+    <row r="424" spans="1:28">
       <c r="A424" t="s">
         <v>1411</v>
       </c>
@@ -33242,7 +33238,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="425" spans="1:28" hidden="1">
+    <row r="425" spans="1:28">
       <c r="A425" t="s">
         <v>1415</v>
       </c>
@@ -33317,7 +33313,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="426" spans="1:28" hidden="1">
+    <row r="426" spans="1:28">
       <c r="A426" t="s">
         <v>1417</v>
       </c>
@@ -33392,7 +33388,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="427" spans="1:28" hidden="1">
+    <row r="427" spans="1:28">
       <c r="A427" t="s">
         <v>1420</v>
       </c>
@@ -33467,7 +33463,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="428" spans="1:28" hidden="1">
+    <row r="428" spans="1:28">
       <c r="A428" t="s">
         <v>1423</v>
       </c>
@@ -33542,7 +33538,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="429" spans="1:28" hidden="1">
+    <row r="429" spans="1:28">
       <c r="A429" t="s">
         <v>1426</v>
       </c>
@@ -33623,7 +33619,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="430" spans="1:28" hidden="1">
+    <row r="430" spans="1:28">
       <c r="A430" t="s">
         <v>1432</v>
       </c>
@@ -33698,7 +33694,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="431" spans="1:28" hidden="1">
+    <row r="431" spans="1:28">
       <c r="A431" t="s">
         <v>1435</v>
       </c>
@@ -33779,7 +33775,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="432" spans="1:28" hidden="1">
+    <row r="432" spans="1:28">
       <c r="A432" t="s">
         <v>1438</v>
       </c>
@@ -33860,7 +33856,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="433" spans="1:28" hidden="1">
+    <row r="433" spans="1:28">
       <c r="A433" t="s">
         <v>1441</v>
       </c>
@@ -33941,7 +33937,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="434" spans="1:28" hidden="1">
+    <row r="434" spans="1:28">
       <c r="A434" t="s">
         <v>1444</v>
       </c>
@@ -34022,7 +34018,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="435" spans="1:28" hidden="1">
+    <row r="435" spans="1:28">
       <c r="A435" t="s">
         <v>1447</v>
       </c>
@@ -34103,7 +34099,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="436" spans="1:28" hidden="1">
+    <row r="436" spans="1:28">
       <c r="A436" t="s">
         <v>1450</v>
       </c>
@@ -34184,7 +34180,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="437" spans="1:28" hidden="1">
+    <row r="437" spans="1:28">
       <c r="A437" t="s">
         <v>1453</v>
       </c>
@@ -34265,7 +34261,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="438" spans="1:28" hidden="1">
+    <row r="438" spans="1:28">
       <c r="A438" t="s">
         <v>1456</v>
       </c>
@@ -34346,7 +34342,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="439" spans="1:28" hidden="1">
+    <row r="439" spans="1:28">
       <c r="A439" t="s">
         <v>1459</v>
       </c>
@@ -34427,7 +34423,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="440" spans="1:28" hidden="1">
+    <row r="440" spans="1:28">
       <c r="A440" t="s">
         <v>1462</v>
       </c>
@@ -34508,7 +34504,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="441" spans="1:28" hidden="1">
+    <row r="441" spans="1:28">
       <c r="A441" t="s">
         <v>1465</v>
       </c>
@@ -34589,7 +34585,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="442" spans="1:28" hidden="1">
+    <row r="442" spans="1:28">
       <c r="D442" t="s">
         <v>1468</v>
       </c>
@@ -34635,7 +34631,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="443" spans="1:28" hidden="1">
+    <row r="443" spans="1:28">
       <c r="D443" t="s">
         <v>1471</v>
       </c>
@@ -34681,7 +34677,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="444" spans="1:28" hidden="1">
+    <row r="444" spans="1:28">
       <c r="D444" t="s">
         <v>1473</v>
       </c>

</xml_diff>